<commit_message>
add notification import excel
</commit_message>
<xml_diff>
--- a/public/downloads/register_students.xlsx
+++ b/public/downloads/register_students.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agil\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\new\Great-Crystal\public\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570B57C-BEF1-4F6C-BAF8-D3E5D2CE4A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFEF4C5-0E8A-4C1B-B56A-09A4974F9BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66309978-6E41-4DD6-9296-E18469648FB4}"/>
   </bookViews>
@@ -235,38 +235,6 @@
   </si>
   <si>
     <r>
-      <t>Student Place of Issue</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Student Date Expiry</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Father Name</t>
     </r>
     <r>
@@ -585,6 +553,12 @@
   </si>
   <si>
     <t>Graduated</t>
+  </si>
+  <si>
+    <t>Student Date Expiry</t>
+  </si>
+  <si>
+    <t>Student Place of Issue</t>
   </si>
 </sst>
 </file>
@@ -962,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FB3641-63C9-4EED-8C17-04F06786AC03}">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,94 +1015,94 @@
         <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -1328,7 +1302,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>